<commit_message>
reduce doc_type name char length
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/doc_type.xlsx
+++ b/mosip_master/xlsx/doc_type.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6350"/>
+    <workbookView windowWidth="19200" windowHeight="6800"/>
   </bookViews>
   <sheets>
     <sheet name="4a1cc61e-b43d-4d06-b7bf-c479afd" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="97">
   <si>
     <t>code</t>
   </si>
@@ -221,39 +221,12 @@
     <t>PDS Card</t>
   </si>
   <si>
-    <t>DOC025</t>
-  </si>
-  <si>
-    <t>Medical card issued by the State Govt, CGHS, ECHS and ESIC</t>
-  </si>
-  <si>
-    <t>Medical card issued by the State Government, CGHS, ECHS and also ESIC</t>
-  </si>
-  <si>
     <t>DOC026</t>
   </si>
   <si>
     <t>Canteen card of the Army</t>
   </si>
   <si>
-    <t>DOC027</t>
-  </si>
-  <si>
-    <t>Family entitlement document</t>
-  </si>
-  <si>
-    <t>Any family entitlement document issued by any Central or State Government</t>
-  </si>
-  <si>
-    <t>DOC028</t>
-  </si>
-  <si>
-    <t>Birth Certificate</t>
-  </si>
-  <si>
-    <t>Registrar of Birth/municipal Corporation or any local government Birth Certificate</t>
-  </si>
-  <si>
     <t>EOP</t>
   </si>
   <si>
@@ -314,12 +287,6 @@
     <t>Licencia de conducir del solicitante</t>
   </si>
   <si>
-    <t>Tarjetas de identificación con fotografía emitidas por el Gobierno.</t>
-  </si>
-  <si>
-    <t>Tarjetas de identificación con fotografía de servicio emitidas por una PSU</t>
-  </si>
-  <si>
     <t>Licencia de Armas</t>
   </si>
   <si>
@@ -344,37 +311,13 @@
     <t>Tarjeta de racionamiento</t>
   </si>
   <si>
-    <t>Tarjeta de identificación con fotografía del servicio emitida por la PSU y dirección</t>
-  </si>
-  <si>
     <t>Factura de luz de los 3 meses anteriores</t>
   </si>
   <si>
-    <t>Factura de agua siempre que no tenga más de 3 meses de antigüedad.</t>
-  </si>
-  <si>
     <t>Tarjeta PDS</t>
   </si>
   <si>
-    <t>Tarjeta médica emitida por el Gobierno del Estado, CGHS, ECHS y ESIC</t>
-  </si>
-  <si>
-    <t>Tarjeta médica emitida por el Gobierno del Estado, CGHS, ECHS y también ESIC</t>
-  </si>
-  <si>
     <t>Tarjeta de comedor del ejército.</t>
-  </si>
-  <si>
-    <t>Documento de derecho familiar</t>
-  </si>
-  <si>
-    <t>Cualquier documento de derecho familiar emitido por cualquier gobierno central o estatal.</t>
-  </si>
-  <si>
-    <t>Certificado de nacimiento</t>
-  </si>
-  <si>
-    <t>Registrador de Nacimiento/Corporación Municipal o cualquier Certificado de Nacimiento del gobierno local</t>
   </si>
   <si>
     <t>Foto de expedición</t>
@@ -1546,17 +1489,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="8.54545454545454" customWidth="1"/>
-    <col min="2" max="2" width="25.9090909090909" customWidth="1"/>
-    <col min="3" max="3" width="25.7272727272727" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="73.9090909090909" customWidth="1"/>
+    <col min="4" max="4" width="36.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2009,7 +1953,7 @@
         <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>7</v>
@@ -2020,13 +1964,13 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>7</v>
@@ -2037,16 +1981,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>8</v>
@@ -2054,16 +1998,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>73</v>
+        <v>9</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>8</v>
@@ -2071,16 +2015,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>75</v>
+        <v>12</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>8</v>
@@ -2088,16 +2032,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>8</v>
@@ -2105,16 +2049,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>8</v>
@@ -2122,16 +2066,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>8</v>
@@ -2139,16 +2083,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>8</v>
@@ -2156,16 +2100,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>8</v>
@@ -2173,16 +2117,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>8</v>
@@ -2190,16 +2134,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>8</v>
@@ -2207,16 +2151,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>8</v>
@@ -2224,16 +2168,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>8</v>
@@ -2241,16 +2185,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>8</v>
@@ -2258,16 +2202,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>8</v>
@@ -2275,16 +2219,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>8</v>
@@ -2292,16 +2236,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>8</v>
@@ -2309,16 +2253,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>8</v>
@@ -2326,16 +2270,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>8</v>
@@ -2343,16 +2287,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>8</v>
@@ -2360,16 +2304,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>8</v>
@@ -2377,16 +2321,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>8</v>
@@ -2394,16 +2338,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>8</v>
@@ -2411,188 +2355,18 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E61" s="2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>